<commit_message>
09/11/24 commit - updated stats sheet - added color legend
</commit_message>
<xml_diff>
--- a/public/results/Bottoms Up 2024 League Stats - Week 19.xlsx
+++ b/public/results/Bottoms Up 2024 League Stats - Week 19.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mthut\iCloudDrive\Golf\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\CODE\golf-league-site\public\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599FA5F9-2AE7-4889-BE7C-D2BB3B351421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10BA088-5008-4EFB-B9F8-F3CE2400DE20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1110" windowWidth="21180" windowHeight="13665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4815" yWindow="1395" windowWidth="21180" windowHeight="13665" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="14" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="134">
   <si>
     <t>Karen</t>
   </si>
@@ -1490,7 +1490,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="224">
+  <cellXfs count="221">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1946,21 +1946,33 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1974,59 +1986,11 @@
     <xf numFmtId="14" fontId="16" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2061,11 +2025,68 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2078,36 +2099,6 @@
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="24" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="18" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2593,23 +2584,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -2623,23 +2614,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -3497,23 +3488,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -3527,23 +3518,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -5171,23 +5162,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -5201,23 +5192,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -6226,23 +6217,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -6256,23 +6247,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -7278,23 +7269,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -7308,23 +7299,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -8715,23 +8706,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -8745,23 +8736,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -9767,23 +9758,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -9797,23 +9788,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -10716,23 +10707,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -10746,23 +10737,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -12082,23 +12073,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -12112,23 +12103,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -13439,24 +13430,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="220" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="213"/>
-      <c r="C1" s="213"/>
-      <c r="D1" s="213"/>
+      <c r="B1" s="220"/>
+      <c r="C1" s="220"/>
+      <c r="D1" s="220"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="213"/>
-      <c r="B2" s="213"/>
-      <c r="C2" s="213"/>
-      <c r="D2" s="213"/>
+      <c r="A2" s="220"/>
+      <c r="B2" s="220"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="213"/>
-      <c r="B3" s="213"/>
-      <c r="C3" s="213"/>
-      <c r="D3" s="213"/>
+      <c r="A3" s="220"/>
+      <c r="B3" s="220"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="220"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -13493,23 +13484,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -13523,23 +13514,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -14841,7 +14832,7 @@
   <dimension ref="A1:BB25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AQ26" sqref="AQ26"/>
+      <selection activeCell="AM25" sqref="AM25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14888,228 +14879,228 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="1" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="197" t="s">
+      <c r="A1" s="185" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="198"/>
-      <c r="C1" s="203"/>
-      <c r="D1" s="206" t="s">
+      <c r="B1" s="186"/>
+      <c r="C1" s="191"/>
+      <c r="D1" s="194" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="175" t="s">
+      <c r="E1" s="179" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="176"/>
-      <c r="G1" s="175" t="s">
+      <c r="F1" s="180"/>
+      <c r="G1" s="179" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="176"/>
-      <c r="I1" s="175" t="s">
+      <c r="H1" s="180"/>
+      <c r="I1" s="179" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="176"/>
-      <c r="K1" s="175" t="s">
+      <c r="J1" s="180"/>
+      <c r="K1" s="179" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="176"/>
-      <c r="M1" s="175" t="s">
+      <c r="L1" s="180"/>
+      <c r="M1" s="179" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="176"/>
-      <c r="O1" s="175" t="s">
+      <c r="N1" s="180"/>
+      <c r="O1" s="179" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="176"/>
-      <c r="Q1" s="175" t="s">
+      <c r="P1" s="180"/>
+      <c r="Q1" s="179" t="s">
         <v>99</v>
       </c>
-      <c r="R1" s="176"/>
-      <c r="S1" s="175" t="s">
+      <c r="R1" s="180"/>
+      <c r="S1" s="179" t="s">
         <v>103</v>
       </c>
-      <c r="T1" s="176"/>
-      <c r="U1" s="175" t="s">
+      <c r="T1" s="180"/>
+      <c r="U1" s="179" t="s">
         <v>107</v>
       </c>
-      <c r="V1" s="176"/>
-      <c r="W1" s="175" t="s">
+      <c r="V1" s="180"/>
+      <c r="W1" s="179" t="s">
         <v>109</v>
       </c>
-      <c r="X1" s="176"/>
-      <c r="Y1" s="175" t="s">
+      <c r="X1" s="180"/>
+      <c r="Y1" s="179" t="s">
         <v>110</v>
       </c>
-      <c r="Z1" s="176"/>
-      <c r="AA1" s="175" t="s">
+      <c r="Z1" s="180"/>
+      <c r="AA1" s="179" t="s">
         <v>119</v>
       </c>
-      <c r="AB1" s="176"/>
-      <c r="AC1" s="175" t="s">
+      <c r="AB1" s="180"/>
+      <c r="AC1" s="179" t="s">
         <v>124</v>
       </c>
-      <c r="AD1" s="176"/>
-      <c r="AE1" s="175" t="s">
+      <c r="AD1" s="180"/>
+      <c r="AE1" s="179" t="s">
         <v>126</v>
       </c>
-      <c r="AF1" s="176"/>
-      <c r="AG1" s="175" t="s">
+      <c r="AF1" s="180"/>
+      <c r="AG1" s="179" t="s">
         <v>127</v>
       </c>
-      <c r="AH1" s="176"/>
-      <c r="AI1" s="175" t="s">
+      <c r="AH1" s="180"/>
+      <c r="AI1" s="179" t="s">
         <v>129</v>
       </c>
-      <c r="AJ1" s="176"/>
-      <c r="AK1" s="175" t="s">
+      <c r="AJ1" s="180"/>
+      <c r="AK1" s="179" t="s">
         <v>130</v>
       </c>
-      <c r="AL1" s="176"/>
-      <c r="AM1" s="175" t="s">
+      <c r="AL1" s="180"/>
+      <c r="AM1" s="179" t="s">
         <v>132</v>
       </c>
-      <c r="AN1" s="176"/>
-      <c r="AO1" s="175" t="s">
+      <c r="AN1" s="180"/>
+      <c r="AO1" s="179" t="s">
         <v>133</v>
       </c>
-      <c r="AP1" s="176"/>
-      <c r="AQ1" s="185" t="s">
+      <c r="AP1" s="180"/>
+      <c r="AQ1" s="196" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="182" t="s">
+      <c r="AR1" s="205" t="s">
         <v>125</v>
       </c>
       <c r="AS1" s="122"/>
-      <c r="AT1" s="188" t="s">
+      <c r="AT1" s="208" t="s">
         <v>117</v>
       </c>
-      <c r="AU1" s="189"/>
-      <c r="AV1" s="189"/>
-      <c r="AW1" s="190"/>
-      <c r="AX1" s="172" t="s">
+      <c r="AU1" s="209"/>
+      <c r="AV1" s="209"/>
+      <c r="AW1" s="210"/>
+      <c r="AX1" s="199" t="s">
         <v>123</v>
       </c>
-      <c r="AY1" s="179" t="s">
+      <c r="AY1" s="202" t="s">
         <v>118</v>
       </c>
-      <c r="AZ1" s="180"/>
-      <c r="BA1" s="180"/>
-      <c r="BB1" s="181"/>
+      <c r="AZ1" s="203"/>
+      <c r="BA1" s="203"/>
+      <c r="BB1" s="204"/>
     </row>
     <row r="2" spans="1:54" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="199"/>
-      <c r="B2" s="200"/>
-      <c r="C2" s="204"/>
-      <c r="D2" s="207"/>
-      <c r="E2" s="177">
+      <c r="A2" s="187"/>
+      <c r="B2" s="188"/>
+      <c r="C2" s="192"/>
+      <c r="D2" s="195"/>
+      <c r="E2" s="181">
         <v>45418</v>
       </c>
-      <c r="F2" s="178"/>
-      <c r="G2" s="208">
+      <c r="F2" s="182"/>
+      <c r="G2" s="183">
         <v>45425</v>
       </c>
-      <c r="H2" s="209"/>
-      <c r="I2" s="208">
+      <c r="H2" s="184"/>
+      <c r="I2" s="183">
         <v>45432</v>
       </c>
-      <c r="J2" s="209"/>
-      <c r="K2" s="208">
+      <c r="J2" s="184"/>
+      <c r="K2" s="183">
         <v>45439</v>
       </c>
-      <c r="L2" s="209"/>
-      <c r="M2" s="208">
+      <c r="L2" s="184"/>
+      <c r="M2" s="183">
         <v>45446</v>
       </c>
-      <c r="N2" s="209"/>
-      <c r="O2" s="208">
+      <c r="N2" s="184"/>
+      <c r="O2" s="183">
         <v>45453</v>
       </c>
-      <c r="P2" s="209"/>
-      <c r="Q2" s="208">
+      <c r="P2" s="184"/>
+      <c r="Q2" s="183">
         <v>45460</v>
       </c>
-      <c r="R2" s="209"/>
-      <c r="S2" s="208">
+      <c r="R2" s="184"/>
+      <c r="S2" s="183">
         <v>45467</v>
       </c>
-      <c r="T2" s="209"/>
-      <c r="U2" s="208">
+      <c r="T2" s="184"/>
+      <c r="U2" s="183">
         <v>45474</v>
       </c>
-      <c r="V2" s="209"/>
-      <c r="W2" s="208">
+      <c r="V2" s="184"/>
+      <c r="W2" s="183">
         <v>45481</v>
       </c>
-      <c r="X2" s="209"/>
-      <c r="Y2" s="208">
+      <c r="X2" s="184"/>
+      <c r="Y2" s="183">
         <v>45488</v>
       </c>
-      <c r="Z2" s="209"/>
-      <c r="AA2" s="177">
+      <c r="Z2" s="184"/>
+      <c r="AA2" s="181">
         <v>45495</v>
       </c>
-      <c r="AB2" s="178"/>
-      <c r="AC2" s="177">
+      <c r="AB2" s="182"/>
+      <c r="AC2" s="181">
         <v>45502</v>
       </c>
-      <c r="AD2" s="178"/>
-      <c r="AE2" s="177">
+      <c r="AD2" s="182"/>
+      <c r="AE2" s="181">
         <v>45509</v>
       </c>
-      <c r="AF2" s="178"/>
-      <c r="AG2" s="177">
+      <c r="AF2" s="182"/>
+      <c r="AG2" s="181">
         <v>45516</v>
       </c>
-      <c r="AH2" s="178"/>
-      <c r="AI2" s="177">
+      <c r="AH2" s="182"/>
+      <c r="AI2" s="181">
         <v>45523</v>
       </c>
-      <c r="AJ2" s="178"/>
-      <c r="AK2" s="177">
+      <c r="AJ2" s="182"/>
+      <c r="AK2" s="181">
         <v>45530</v>
       </c>
-      <c r="AL2" s="178"/>
-      <c r="AM2" s="177">
+      <c r="AL2" s="182"/>
+      <c r="AM2" s="181">
         <v>45537</v>
       </c>
-      <c r="AN2" s="178"/>
-      <c r="AO2" s="177">
+      <c r="AN2" s="182"/>
+      <c r="AO2" s="181">
         <v>45544</v>
       </c>
-      <c r="AP2" s="178"/>
-      <c r="AQ2" s="186"/>
-      <c r="AR2" s="183"/>
+      <c r="AP2" s="182"/>
+      <c r="AQ2" s="197"/>
+      <c r="AR2" s="206"/>
       <c r="AS2" s="122"/>
-      <c r="AT2" s="191" t="s">
+      <c r="AT2" s="211" t="s">
         <v>98</v>
       </c>
-      <c r="AU2" s="193" t="s">
+      <c r="AU2" s="213" t="s">
         <v>116</v>
       </c>
-      <c r="AV2" s="193" t="s">
+      <c r="AV2" s="213" t="s">
         <v>43</v>
       </c>
-      <c r="AW2" s="195" t="s">
+      <c r="AW2" s="215" t="s">
         <v>70</v>
       </c>
-      <c r="AX2" s="173"/>
-      <c r="AY2" s="172" t="s">
+      <c r="AX2" s="200"/>
+      <c r="AY2" s="199" t="s">
         <v>98</v>
       </c>
-      <c r="AZ2" s="172" t="s">
+      <c r="AZ2" s="199" t="s">
         <v>116</v>
       </c>
-      <c r="BA2" s="172" t="s">
+      <c r="BA2" s="199" t="s">
         <v>43</v>
       </c>
-      <c r="BB2" s="172" t="s">
+      <c r="BB2" s="199" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:54" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="201"/>
-      <c r="B3" s="202"/>
-      <c r="C3" s="205"/>
-      <c r="D3" s="207"/>
+      <c r="A3" s="189"/>
+      <c r="B3" s="190"/>
+      <c r="C3" s="193"/>
+      <c r="D3" s="195"/>
       <c r="E3" s="60" t="s">
         <v>28</v>
       </c>
@@ -15224,18 +15215,18 @@
       <c r="AP3" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="AQ3" s="187"/>
-      <c r="AR3" s="184"/>
+      <c r="AQ3" s="198"/>
+      <c r="AR3" s="207"/>
       <c r="AS3" s="122"/>
-      <c r="AT3" s="192"/>
-      <c r="AU3" s="194"/>
-      <c r="AV3" s="194"/>
-      <c r="AW3" s="196"/>
-      <c r="AX3" s="174"/>
-      <c r="AY3" s="173"/>
-      <c r="AZ3" s="173"/>
-      <c r="BA3" s="173"/>
-      <c r="BB3" s="174"/>
+      <c r="AT3" s="212"/>
+      <c r="AU3" s="214"/>
+      <c r="AV3" s="214"/>
+      <c r="AW3" s="216"/>
+      <c r="AX3" s="201"/>
+      <c r="AY3" s="200"/>
+      <c r="AZ3" s="200"/>
+      <c r="BA3" s="200"/>
+      <c r="BB3" s="201"/>
     </row>
     <row r="4" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
@@ -15248,7 +15239,7 @@
         <v>40</v>
       </c>
       <c r="D4" s="67">
-        <f>ROUND(AR4-36,2)</f>
+        <f t="shared" ref="D4:D16" si="0">ROUND(AR4-36,2)</f>
         <v>12.2</v>
       </c>
       <c r="E4" s="160">
@@ -15347,14 +15338,14 @@
       <c r="AN4" s="78">
         <v>26</v>
       </c>
-      <c r="AO4" s="214"/>
-      <c r="AP4" s="215"/>
+      <c r="AO4" s="169"/>
+      <c r="AP4" s="170"/>
       <c r="AQ4" s="71">
-        <f>SUMIF(E4:AO4,"&gt;30")</f>
+        <f t="shared" ref="AQ4:AQ20" si="1">SUMIF(E4:AO4,"&gt;30")</f>
         <v>723</v>
       </c>
       <c r="AR4" s="72">
-        <f>AQ4/(AT4+AY4)</f>
+        <f t="shared" ref="AR4:AR20" si="2">AQ4/(AT4+AY4)</f>
         <v>48.2</v>
       </c>
       <c r="AS4" s="112"/>
@@ -15377,18 +15368,18 @@
         <v>122</v>
       </c>
       <c r="AY4" s="140">
-        <f>COUNTIF(AA4:AO4, "&gt;30")</f>
-        <v>4</v>
-      </c>
-      <c r="AZ4" s="218">
+        <f t="shared" ref="AY4:AY20" si="3">COUNTIF(AA4:AO4, "&gt;30")</f>
+        <v>4</v>
+      </c>
+      <c r="AZ4" s="171">
         <v>3</v>
       </c>
       <c r="BA4" s="140">
-        <f>SUMIF(AB4:AP4, "&lt;30")+AZ4</f>
+        <f t="shared" ref="BA4:BA20" si="4">SUMIF(AB4:AP4, "&lt;30")+AZ4</f>
         <v>86</v>
       </c>
       <c r="BB4" s="151">
-        <f>(BA4)/AY4</f>
+        <f t="shared" ref="BB4:BB15" si="5">(BA4)/AY4</f>
         <v>21.5</v>
       </c>
     </row>
@@ -15403,7 +15394,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="76">
-        <f>ROUND(AR5-36,2)</f>
+        <f t="shared" si="0"/>
         <v>14.46</v>
       </c>
       <c r="E5" s="77">
@@ -15490,18 +15481,18 @@
       </c>
       <c r="AM5" s="79"/>
       <c r="AN5" s="80"/>
-      <c r="AO5" s="216">
+      <c r="AO5" s="77">
         <v>47</v>
       </c>
-      <c r="AP5" s="217">
+      <c r="AP5" s="78">
         <v>22</v>
       </c>
       <c r="AQ5" s="71">
-        <f>SUMIF(E5:AO5,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>656</v>
       </c>
       <c r="AR5" s="72">
-        <f>AQ5/(AT5+AY5)</f>
+        <f t="shared" si="2"/>
         <v>50.46153846153846</v>
       </c>
       <c r="AS5" s="112"/>
@@ -15522,18 +15513,18 @@
       </c>
       <c r="AX5" s="144"/>
       <c r="AY5" s="149">
-        <f>COUNTIF(AA5:AO5, "&gt;30")</f>
-        <v>4</v>
-      </c>
-      <c r="AZ5" s="219">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AZ5" s="172">
         <v>0</v>
       </c>
       <c r="BA5" s="149">
-        <f>SUMIF(AB5:AP5, "&lt;30")+AZ5</f>
+        <f t="shared" si="4"/>
         <v>86</v>
       </c>
       <c r="BB5" s="152">
-        <f>(BA5)/AY5</f>
+        <f t="shared" si="5"/>
         <v>21.5</v>
       </c>
     </row>
@@ -15548,7 +15539,7 @@
         <v>40</v>
       </c>
       <c r="D6" s="76">
-        <f>ROUND(AR6-36,2)</f>
+        <f t="shared" si="0"/>
         <v>1.77</v>
       </c>
       <c r="E6" s="77">
@@ -15585,7 +15576,7 @@
       </c>
       <c r="Q6" s="82"/>
       <c r="R6" s="80"/>
-      <c r="S6" s="221">
+      <c r="S6" s="174">
         <v>38</v>
       </c>
       <c r="T6" s="78">
@@ -15635,18 +15626,18 @@
       <c r="AN6" s="78">
         <v>18</v>
       </c>
-      <c r="AO6" s="222">
+      <c r="AO6" s="175">
         <v>34</v>
       </c>
       <c r="AP6" s="78">
         <v>22</v>
       </c>
       <c r="AQ6" s="71">
-        <f>SUMIF(E6:AO6,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>491</v>
       </c>
       <c r="AR6" s="72">
-        <f>AQ6/(AT6+AY6)</f>
+        <f t="shared" si="2"/>
         <v>37.769230769230766</v>
       </c>
       <c r="AS6" s="112"/>
@@ -15667,18 +15658,18 @@
       </c>
       <c r="AX6" s="145"/>
       <c r="AY6" s="149">
-        <f>COUNTIF(AA6:AO6, "&gt;30")</f>
-        <v>6</v>
-      </c>
-      <c r="AZ6" s="219">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="AZ6" s="172">
         <v>6</v>
       </c>
       <c r="BA6" s="149">
-        <f>SUMIF(AB6:AP6, "&lt;30")+AZ6</f>
+        <f t="shared" si="4"/>
         <v>117</v>
       </c>
       <c r="BB6" s="152">
-        <f>(BA6)/AY6</f>
+        <f t="shared" si="5"/>
         <v>19.5</v>
       </c>
     </row>
@@ -15693,7 +15684,7 @@
         <v>40</v>
       </c>
       <c r="D7" s="76">
-        <f>ROUND(AR7-36,2)</f>
+        <f t="shared" si="0"/>
         <v>21.11</v>
       </c>
       <c r="E7" s="77">
@@ -15768,18 +15759,18 @@
       </c>
       <c r="AM7" s="79"/>
       <c r="AN7" s="80"/>
-      <c r="AO7" s="223">
+      <c r="AO7" s="111">
         <v>61</v>
       </c>
-      <c r="AP7" s="217">
+      <c r="AP7" s="78">
         <v>14</v>
       </c>
       <c r="AQ7" s="71">
-        <f>SUMIF(E7:AO7,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>514</v>
       </c>
       <c r="AR7" s="72">
-        <f>AQ7/(AT7+AY7)</f>
+        <f t="shared" si="2"/>
         <v>57.111111111111114</v>
       </c>
       <c r="AS7" s="112"/>
@@ -15800,18 +15791,18 @@
       </c>
       <c r="AX7" s="144"/>
       <c r="AY7" s="149">
-        <f>COUNTIF(AA7:AO7, "&gt;30")</f>
-        <v>3</v>
-      </c>
-      <c r="AZ7" s="219">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="AZ7" s="172">
         <v>0</v>
       </c>
       <c r="BA7" s="149">
-        <f>SUMIF(AB7:AP7, "&lt;30")+AZ7</f>
+        <f t="shared" si="4"/>
         <v>57</v>
       </c>
       <c r="BB7" s="152">
-        <f>(BA7)/AY7</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
     </row>
@@ -15826,7 +15817,7 @@
         <v>115</v>
       </c>
       <c r="D8" s="76">
-        <f>ROUND(AR8-36,2)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="E8" s="79"/>
@@ -15877,18 +15868,18 @@
       <c r="AL8" s="80"/>
       <c r="AM8" s="79"/>
       <c r="AN8" s="80"/>
-      <c r="AO8" s="216">
+      <c r="AO8" s="77">
         <v>56</v>
       </c>
-      <c r="AP8" s="217">
+      <c r="AP8" s="78">
         <v>21</v>
       </c>
       <c r="AQ8" s="71">
-        <f>SUMIF(E8:AO8,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>232</v>
       </c>
       <c r="AR8" s="72">
-        <f>AQ8/(AT8+AY8)</f>
+        <f t="shared" si="2"/>
         <v>58</v>
       </c>
       <c r="AS8" s="112"/>
@@ -15906,18 +15897,18 @@
       </c>
       <c r="AX8" s="145"/>
       <c r="AY8" s="149">
-        <f>COUNTIF(AA8:AO8, "&gt;30")</f>
-        <v>4</v>
-      </c>
-      <c r="AZ8" s="219">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AZ8" s="172">
         <v>0</v>
       </c>
       <c r="BA8" s="149">
-        <f>SUMIF(AB8:AP8, "&lt;30")+AZ8</f>
+        <f t="shared" si="4"/>
         <v>76</v>
       </c>
       <c r="BB8" s="152">
-        <f>(BA8)/AY8</f>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
     </row>
@@ -15932,7 +15923,7 @@
         <v>40</v>
       </c>
       <c r="D9" s="76">
-        <f>ROUND(AR9-36,2)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E9" s="77">
@@ -16026,43 +16017,43 @@
         <v>19</v>
       </c>
       <c r="AQ9" s="71">
-        <f>SUMIF(E9:AO9,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>585</v>
       </c>
       <c r="AR9" s="72">
-        <f>AQ9/(AT9+AY9)</f>
+        <f t="shared" si="2"/>
         <v>45</v>
       </c>
       <c r="AS9" s="112"/>
       <c r="AT9" s="81">
-        <f>COUNTIF(E9:Y9,"&gt;30")</f>
+        <f t="shared" ref="AT9:AT20" si="6">COUNTIF(E9:Y9,"&gt;30")</f>
         <v>7</v>
       </c>
       <c r="AU9" s="114">
         <v>2</v>
       </c>
       <c r="AV9" s="115">
-        <f>SUMIF(E9:Z9,"&lt;30")+AU9</f>
+        <f t="shared" ref="AV9:AV20" si="7">SUMIF(E9:Z9,"&lt;30")+AU9</f>
         <v>126</v>
       </c>
       <c r="AW9" s="124">
-        <f>(AV9)/AT9</f>
+        <f t="shared" ref="AW9:AW20" si="8">(AV9)/AT9</f>
         <v>18</v>
       </c>
       <c r="AX9" s="145"/>
       <c r="AY9" s="149">
-        <f>COUNTIF(AA9:AO9, "&gt;30")</f>
-        <v>6</v>
-      </c>
-      <c r="AZ9" s="219">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="AZ9" s="172">
         <v>1</v>
       </c>
       <c r="BA9" s="149">
-        <f>SUMIF(AB9:AP9, "&lt;30")+AZ9</f>
+        <f t="shared" si="4"/>
         <v>111</v>
       </c>
       <c r="BB9" s="152">
-        <f>(BA9)/AY9</f>
+        <f t="shared" si="5"/>
         <v>18.5</v>
       </c>
     </row>
@@ -16077,7 +16068,7 @@
         <v>40</v>
       </c>
       <c r="D10" s="76">
-        <f>ROUND(AR10-36,2)</f>
+        <f t="shared" si="0"/>
         <v>12.5</v>
       </c>
       <c r="E10" s="77">
@@ -16167,43 +16158,43 @@
         <v>21</v>
       </c>
       <c r="AQ10" s="71">
-        <f>SUMIF(E10:AO10,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>582</v>
       </c>
       <c r="AR10" s="72">
-        <f>AQ10/(AT10+AY10)</f>
+        <f t="shared" si="2"/>
         <v>48.5</v>
       </c>
       <c r="AS10" s="112"/>
       <c r="AT10" s="81">
-        <f>COUNTIF(E10:Y10,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="AU10" s="114">
         <v>2</v>
       </c>
       <c r="AV10" s="115">
-        <f>SUMIF(E10:Z10,"&lt;30")+AU10</f>
+        <f t="shared" si="7"/>
         <v>127</v>
       </c>
       <c r="AW10" s="124">
-        <f>(AV10)/AT10</f>
+        <f t="shared" si="8"/>
         <v>18.142857142857142</v>
       </c>
       <c r="AX10" s="145"/>
       <c r="AY10" s="149">
-        <f>COUNTIF(AA10:AO10, "&gt;30")</f>
-        <v>5</v>
-      </c>
-      <c r="AZ10" s="219">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="AZ10" s="172">
         <v>0</v>
       </c>
       <c r="BA10" s="149">
-        <f>SUMIF(AB10:AP10, "&lt;30")+AZ10</f>
+        <f t="shared" si="4"/>
         <v>91</v>
       </c>
       <c r="BB10" s="152">
-        <f>(BA10)/AY10</f>
+        <f t="shared" si="5"/>
         <v>18.2</v>
       </c>
     </row>
@@ -16218,7 +16209,7 @@
         <v>115</v>
       </c>
       <c r="D11" s="76">
-        <f>ROUND(AR11-36,2)</f>
+        <f t="shared" si="0"/>
         <v>15.14</v>
       </c>
       <c r="E11" s="79"/>
@@ -16288,43 +16279,43 @@
       <c r="AO11" s="79"/>
       <c r="AP11" s="80"/>
       <c r="AQ11" s="71">
-        <f>SUMIF(E11:AO11,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>358</v>
       </c>
       <c r="AR11" s="72">
-        <f>AQ11/(AT11+AY11)</f>
+        <f t="shared" si="2"/>
         <v>51.142857142857146</v>
       </c>
       <c r="AS11" s="112"/>
       <c r="AT11" s="81">
-        <f>COUNTIF(E11:Y11,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="AU11" s="114">
         <v>0</v>
       </c>
       <c r="AV11" s="115">
-        <f>SUMIF(E11:Z11,"&lt;30")+AU11</f>
+        <f t="shared" si="7"/>
         <v>88</v>
       </c>
       <c r="AW11" s="124">
-        <f>(AV11)/AT11</f>
+        <f t="shared" si="8"/>
         <v>17.600000000000001</v>
       </c>
       <c r="AX11" s="145"/>
       <c r="AY11" s="149">
-        <f>COUNTIF(AA11:AO11, "&gt;30")</f>
-        <v>2</v>
-      </c>
-      <c r="AZ11" s="219">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="AZ11" s="172">
         <v>0</v>
       </c>
       <c r="BA11" s="149">
-        <f>SUMIF(AB11:AP11, "&lt;30")+AZ11</f>
+        <f t="shared" si="4"/>
         <v>36</v>
       </c>
       <c r="BB11" s="152">
-        <f>(BA11)/AY11</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
@@ -16339,7 +16330,7 @@
         <v>40</v>
       </c>
       <c r="D12" s="76">
-        <f>ROUND(AR12-36,2)</f>
+        <f t="shared" si="0"/>
         <v>14.56</v>
       </c>
       <c r="E12" s="77">
@@ -16445,45 +16436,45 @@
         <v>21</v>
       </c>
       <c r="AQ12" s="71">
-        <f>SUMIF(E12:AO12,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>809</v>
       </c>
       <c r="AR12" s="72">
-        <f>AQ12/(AT12+AY12)</f>
+        <f t="shared" si="2"/>
         <v>50.5625</v>
       </c>
       <c r="AS12" s="112"/>
       <c r="AT12" s="81">
-        <f>COUNTIF(E12:Y12,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
       <c r="AU12" s="114">
         <v>1</v>
       </c>
       <c r="AV12" s="115">
-        <f>SUMIF(E12:Z12,"&lt;30")+AU12</f>
+        <f t="shared" si="7"/>
         <v>189</v>
       </c>
       <c r="AW12" s="124">
-        <f>(AV12)/AT12</f>
+        <f t="shared" si="8"/>
         <v>18.899999999999999</v>
       </c>
       <c r="AX12" s="146" t="s">
         <v>121</v>
       </c>
       <c r="AY12" s="149">
-        <f>COUNTIF(AA12:AO12, "&gt;30")</f>
-        <v>6</v>
-      </c>
-      <c r="AZ12" s="219">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="AZ12" s="172">
         <v>0</v>
       </c>
       <c r="BA12" s="149">
-        <f>SUMIF(AB12:AP12, "&lt;30")+AZ12</f>
+        <f t="shared" si="4"/>
         <v>105</v>
       </c>
       <c r="BB12" s="152">
-        <f>(BA12)/AY12</f>
+        <f t="shared" si="5"/>
         <v>17.5</v>
       </c>
     </row>
@@ -16498,7 +16489,7 @@
         <v>40</v>
       </c>
       <c r="D13" s="76">
-        <f>ROUND(AR13-36,2)</f>
+        <f t="shared" si="0"/>
         <v>11.09</v>
       </c>
       <c r="E13" s="79"/>
@@ -16584,45 +16575,45 @@
       <c r="AO13" s="79"/>
       <c r="AP13" s="80"/>
       <c r="AQ13" s="71">
-        <f>SUMIF(E13:AO13,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>518</v>
       </c>
       <c r="AR13" s="72">
-        <f>AQ13/(AT13+AY13)</f>
+        <f t="shared" si="2"/>
         <v>47.090909090909093</v>
       </c>
       <c r="AS13" s="112"/>
       <c r="AT13" s="81">
-        <f>COUNTIF(E13:Y13,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="AU13" s="114">
         <v>2</v>
       </c>
       <c r="AV13" s="115">
-        <f>SUMIF(E13:Z13,"&lt;30")+AU13</f>
+        <f t="shared" si="7"/>
         <v>115</v>
       </c>
       <c r="AW13" s="124">
-        <f>(AV13)/AT13</f>
+        <f t="shared" si="8"/>
         <v>19.166666666666668</v>
       </c>
       <c r="AX13" s="146" t="s">
         <v>120</v>
       </c>
       <c r="AY13" s="149">
-        <f>COUNTIF(AA13:AO13, "&gt;30")</f>
-        <v>5</v>
-      </c>
-      <c r="AZ13" s="219">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="AZ13" s="172">
         <v>1</v>
       </c>
       <c r="BA13" s="149">
-        <f>SUMIF(AB13:AP13, "&lt;30")+AZ13</f>
+        <f t="shared" si="4"/>
         <v>85</v>
       </c>
       <c r="BB13" s="152">
-        <f>(BA13)/AY13</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
     </row>
@@ -16637,7 +16628,7 @@
         <v>40</v>
       </c>
       <c r="D14" s="76">
-        <f>ROUND(AR14-36,2)</f>
+        <f t="shared" si="0"/>
         <v>21.47</v>
       </c>
       <c r="E14" s="77">
@@ -16739,43 +16730,43 @@
         <v>12</v>
       </c>
       <c r="AQ14" s="71">
-        <f>SUMIF(E14:AO14,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>862</v>
       </c>
       <c r="AR14" s="72">
-        <f>AQ14/(AT14+AY14)</f>
+        <f t="shared" si="2"/>
         <v>57.466666666666669</v>
       </c>
       <c r="AS14" s="112"/>
       <c r="AT14" s="81">
-        <f>COUNTIF(E14:Y14,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="AU14" s="114">
         <v>0</v>
       </c>
       <c r="AV14" s="115">
-        <f>SUMIF(E14:Z14,"&lt;30")+AU14</f>
+        <f t="shared" si="7"/>
         <v>166</v>
       </c>
       <c r="AW14" s="124">
-        <f>(AV14)/AT14</f>
+        <f t="shared" si="8"/>
         <v>18.444444444444443</v>
       </c>
       <c r="AX14" s="145"/>
       <c r="AY14" s="149">
-        <f>COUNTIF(AA14:AO14, "&gt;30")</f>
-        <v>6</v>
-      </c>
-      <c r="AZ14" s="219">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="AZ14" s="172">
         <v>0</v>
       </c>
       <c r="BA14" s="149">
-        <f>SUMIF(AB14:AP14, "&lt;30")+AZ14</f>
+        <f t="shared" si="4"/>
         <v>101</v>
       </c>
       <c r="BB14" s="152">
-        <f>(BA14)/AY14</f>
+        <f t="shared" si="5"/>
         <v>16.833333333333332</v>
       </c>
     </row>
@@ -16790,7 +16781,7 @@
         <v>40</v>
       </c>
       <c r="D15" s="76">
-        <f>ROUND(AR15-36,2)</f>
+        <f t="shared" si="0"/>
         <v>16.670000000000002</v>
       </c>
       <c r="E15" s="77">
@@ -16880,43 +16871,43 @@
       <c r="AO15" s="79"/>
       <c r="AP15" s="80"/>
       <c r="AQ15" s="71">
-        <f>SUMIF(E15:AO15,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>632</v>
       </c>
       <c r="AR15" s="72">
-        <f>AQ15/(AT15+AY15)</f>
+        <f t="shared" si="2"/>
         <v>52.666666666666664</v>
       </c>
       <c r="AS15" s="112"/>
       <c r="AT15" s="81">
-        <f>COUNTIF(E15:Y15,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="AU15" s="114">
         <v>0</v>
       </c>
       <c r="AV15" s="115">
-        <f>SUMIF(E15:Z15,"&lt;30")+AU15</f>
+        <f t="shared" si="7"/>
         <v>146</v>
       </c>
       <c r="AW15" s="124">
-        <f>(AV15)/AT15</f>
+        <f t="shared" si="8"/>
         <v>18.25</v>
       </c>
       <c r="AX15" s="145"/>
       <c r="AY15" s="149">
-        <f>COUNTIF(AA15:AO15, "&gt;30")</f>
-        <v>4</v>
-      </c>
-      <c r="AZ15" s="219">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AZ15" s="172">
         <v>1</v>
       </c>
       <c r="BA15" s="149">
-        <f>SUMIF(AB15:AP15, "&lt;30")+AZ15</f>
+        <f t="shared" si="4"/>
         <v>66</v>
       </c>
       <c r="BB15" s="152">
-        <f>(BA15)/AY15</f>
+        <f t="shared" si="5"/>
         <v>16.5</v>
       </c>
     </row>
@@ -16931,7 +16922,7 @@
         <v>40</v>
       </c>
       <c r="D16" s="76">
-        <f>ROUND(AR16-36,2)</f>
+        <f t="shared" si="0"/>
         <v>8.33</v>
       </c>
       <c r="E16" s="77">
@@ -17015,39 +17006,39 @@
       <c r="AO16" s="79"/>
       <c r="AP16" s="80"/>
       <c r="AQ16" s="71">
-        <f>SUMIF(E16:AO16,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>399</v>
       </c>
       <c r="AR16" s="72">
-        <f>AQ16/(AT16+AY16)</f>
+        <f t="shared" si="2"/>
         <v>44.333333333333336</v>
       </c>
       <c r="AS16" s="112"/>
       <c r="AT16" s="81">
-        <f>COUNTIF(E16:Y16,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="AU16" s="114">
         <v>1</v>
       </c>
       <c r="AV16" s="115">
-        <f>SUMIF(E16:Z16,"&lt;30")+AU16</f>
+        <f t="shared" si="7"/>
         <v>169</v>
       </c>
       <c r="AW16" s="124">
-        <f>(AV16)/AT16</f>
+        <f t="shared" si="8"/>
         <v>18.777777777777779</v>
       </c>
       <c r="AX16" s="147"/>
       <c r="AY16" s="149">
-        <f>COUNTIF(AA16:AO16, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AZ16" s="219">
+      <c r="AZ16" s="172">
         <v>0</v>
       </c>
       <c r="BA16" s="149">
-        <f>SUMIF(AB16:AP16, "&lt;30")+AZ16</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BB16" s="152">
@@ -17110,39 +17101,39 @@
       <c r="AO17" s="79"/>
       <c r="AP17" s="80"/>
       <c r="AQ17" s="71">
-        <f>SUMIF(E17:AO17,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="AR17" s="72">
-        <f>AQ17/(AT17+AY17)</f>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="AS17" s="112"/>
       <c r="AT17" s="81">
-        <f>COUNTIF(E17:Y17,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AU17" s="114">
         <v>0</v>
       </c>
       <c r="AV17" s="115">
-        <f>SUMIF(E17:Z17,"&lt;30")+AU17</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AW17" s="124">
-        <f>(AV17)/AT17</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AX17" s="145"/>
       <c r="AY17" s="149">
-        <f>COUNTIF(AA17:AO17, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AZ17" s="219">
+      <c r="AZ17" s="172">
         <v>0</v>
       </c>
       <c r="BA17" s="149">
-        <f>SUMIF(AB17:AP17, "&lt;30")+AZ17</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BB17" s="152">
@@ -17205,39 +17196,39 @@
       <c r="AO18" s="79"/>
       <c r="AP18" s="80"/>
       <c r="AQ18" s="71">
-        <f>SUMIF(E18:AO18,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="AR18" s="72">
-        <f>AQ18/(AT18+AY18)</f>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="AS18" s="112"/>
       <c r="AT18" s="81">
-        <f>COUNTIF(E18:Y18,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AU18" s="115">
         <v>0</v>
       </c>
       <c r="AV18" s="115">
-        <f>SUMIF(E18:Z18,"&lt;30")+AU18</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AW18" s="124">
-        <f>(AV18)/AT18</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AX18" s="145"/>
       <c r="AY18" s="149">
-        <f>COUNTIF(AA18:AO18, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AZ18" s="149">
         <v>0</v>
       </c>
       <c r="BA18" s="149">
-        <f>SUMIF(AB18:AP18, "&lt;30")+AZ18</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BB18" s="152">
@@ -17313,39 +17304,39 @@
       <c r="AO19" s="79"/>
       <c r="AP19" s="80"/>
       <c r="AQ19" s="71">
-        <f>SUMIF(E19:AO19,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>217</v>
       </c>
       <c r="AR19" s="72">
-        <f>AQ19/(AT19+AY19)</f>
+        <f t="shared" si="2"/>
         <v>54.25</v>
       </c>
       <c r="AS19" s="112"/>
       <c r="AT19" s="81">
-        <f>COUNTIF(E19:Y19,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="AU19" s="114">
         <v>0</v>
       </c>
       <c r="AV19" s="115">
-        <f>SUMIF(E19:Z19,"&lt;30")+AU19</f>
+        <f t="shared" si="7"/>
         <v>72</v>
       </c>
       <c r="AW19" s="124">
-        <f>(AV19)/AT19</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="AX19" s="145"/>
       <c r="AY19" s="149">
-        <f>COUNTIF(AA19:AO19, "&gt;30")</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AZ19" s="219">
+      <c r="AZ19" s="172">
         <v>0</v>
       </c>
       <c r="BA19" s="149">
-        <f>SUMIF(AB19:AP19, "&lt;30")+AZ19</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BB19" s="152">
@@ -17412,39 +17403,39 @@
       <c r="AO20" s="79"/>
       <c r="AP20" s="80"/>
       <c r="AQ20" s="71">
-        <f>SUMIF(E20:AO20,"&gt;30")</f>
+        <f t="shared" si="1"/>
         <v>123</v>
       </c>
       <c r="AR20" s="72">
-        <f>AQ20/(AT20+AY20)</f>
+        <f t="shared" si="2"/>
         <v>61.5</v>
       </c>
       <c r="AS20" s="112"/>
       <c r="AT20" s="125">
-        <f>COUNTIF(E20:Y20,"&gt;30")</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="AU20" s="116">
         <v>0</v>
       </c>
       <c r="AV20" s="130">
-        <f>SUMIF(E20:Z20,"&lt;30")+AU20</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AW20" s="131">
-        <f>(AV20)/AT20</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AX20" s="148"/>
       <c r="AY20" s="150">
-        <f>COUNTIF(AA20:AO20, "&gt;30")</f>
-        <v>1</v>
-      </c>
-      <c r="AZ20" s="220">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AZ20" s="173">
         <v>0</v>
       </c>
       <c r="BA20" s="150">
-        <f>SUMIF(AB20:AP20, "&lt;30")+AZ20</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BB20" s="153">
@@ -17586,7 +17577,9 @@
       <c r="AK23" s="133" t="s">
         <v>32</v>
       </c>
-      <c r="AM23" s="133"/>
+      <c r="AM23" s="133" t="s">
+        <v>32</v>
+      </c>
       <c r="AO23" s="133"/>
     </row>
     <row r="24" spans="1:54" x14ac:dyDescent="0.25">
@@ -17608,7 +17601,9 @@
       <c r="AK24" s="132" t="s">
         <v>33</v>
       </c>
-      <c r="AM24" s="132"/>
+      <c r="AM24" s="132" t="s">
+        <v>33</v>
+      </c>
       <c r="AO24" s="132"/>
     </row>
     <row r="25" spans="1:54" x14ac:dyDescent="0.25">
@@ -17630,7 +17625,9 @@
         <v>105</v>
       </c>
       <c r="AL25" s="143"/>
-      <c r="AM25" s="134"/>
+      <c r="AM25" s="134" t="s">
+        <v>105</v>
+      </c>
       <c r="AN25" s="143"/>
       <c r="AO25" s="134"/>
       <c r="AP25" s="143"/>
@@ -17641,6 +17638,44 @@
     <sortCondition ref="AR4:AR20"/>
   </sortState>
   <mergeCells count="54">
+    <mergeCell ref="AX1:AX3"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AY1:BB1"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="AR1:AR3"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AT2:AT3"/>
+    <mergeCell ref="AU2:AU3"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AQ1:AQ3"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="E2:F2"/>
@@ -17657,44 +17692,6 @@
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AQ1:AQ3"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AX1:AX3"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AY1:BB1"/>
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BA2:BA3"/>
-    <mergeCell ref="BB2:BB3"/>
-    <mergeCell ref="AR1:AR3"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AT2:AT3"/>
-    <mergeCell ref="AU2:AU3"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AW2:AW3"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17719,24 +17716,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="213" t="s">
+      <c r="A1" s="220" t="s">
         <v>131</v>
       </c>
-      <c r="B1" s="213"/>
-      <c r="C1" s="213"/>
-      <c r="D1" s="213"/>
+      <c r="B1" s="220"/>
+      <c r="C1" s="220"/>
+      <c r="D1" s="220"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="213"/>
-      <c r="B2" s="213"/>
-      <c r="C2" s="213"/>
-      <c r="D2" s="213"/>
+      <c r="A2" s="220"/>
+      <c r="B2" s="220"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="213"/>
-      <c r="B3" s="213"/>
-      <c r="C3" s="213"/>
-      <c r="D3" s="213"/>
+      <c r="A3" s="220"/>
+      <c r="B3" s="220"/>
+      <c r="C3" s="220"/>
+      <c r="D3" s="220"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -17773,23 +17770,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -17803,23 +17800,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -19143,23 +19140,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -19173,23 +19170,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -20466,23 +20463,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -20496,23 +20493,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -23410,23 +23407,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -23440,23 +23437,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -24982,23 +24979,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -25012,23 +25009,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -26643,23 +26640,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -26673,23 +26670,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -28095,23 +28092,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -28125,23 +28122,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -29490,23 +29487,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="176" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="170"/>
-      <c r="C1" s="170"/>
-      <c r="D1" s="170"/>
-      <c r="E1" s="170"/>
-      <c r="F1" s="170"/>
-      <c r="G1" s="170"/>
-      <c r="H1" s="170"/>
-      <c r="I1" s="170"/>
-      <c r="J1" s="170"/>
-      <c r="K1" s="170"/>
-      <c r="L1" s="170"/>
-      <c r="M1" s="170"/>
-      <c r="N1" s="170"/>
-      <c r="O1" s="170"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
+      <c r="G1" s="177"/>
+      <c r="H1" s="177"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="177"/>
+      <c r="K1" s="177"/>
+      <c r="L1" s="177"/>
+      <c r="M1" s="177"/>
+      <c r="N1" s="177"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
@@ -29520,23 +29517,23 @@
       <c r="Z1" s="12"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="171" t="s">
+      <c r="A2" s="178" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
-      <c r="G2" s="170"/>
-      <c r="H2" s="170"/>
-      <c r="I2" s="170"/>
-      <c r="J2" s="170"/>
-      <c r="K2" s="170"/>
-      <c r="L2" s="170"/>
-      <c r="M2" s="170"/>
-      <c r="N2" s="170"/>
-      <c r="O2" s="170"/>
+      <c r="B2" s="177"/>
+      <c r="C2" s="177"/>
+      <c r="D2" s="177"/>
+      <c r="E2" s="177"/>
+      <c r="F2" s="177"/>
+      <c r="G2" s="177"/>
+      <c r="H2" s="177"/>
+      <c r="I2" s="177"/>
+      <c r="J2" s="177"/>
+      <c r="K2" s="177"/>
+      <c r="L2" s="177"/>
+      <c r="M2" s="177"/>
+      <c r="N2" s="177"/>
+      <c r="O2" s="177"/>
       <c r="P2" s="12"/>
       <c r="Q2" s="12"/>
       <c r="R2" s="12"/>
@@ -30293,9 +30290,9 @@
       </c>
       <c r="O15" s="25"/>
       <c r="P15" s="46"/>
-      <c r="Q15" s="210"/>
-      <c r="R15" s="211"/>
-      <c r="S15" s="212"/>
+      <c r="Q15" s="217"/>
+      <c r="R15" s="218"/>
+      <c r="S15" s="219"/>
       <c r="T15" s="51">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
09/11/24 commit - further styling of hover over images.  changed overall standings pdf to landscape layout
</commit_message>
<xml_diff>
--- a/public/results/Bottoms Up 2024 League Stats - Week 19.xlsx
+++ b/public/results/Bottoms Up 2024 League Stats - Week 19.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DATA\CODE\golf-league-site\public\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24EDEB9E-CA6D-415F-9292-366F6E60C42D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9881031A-2708-4049-B37D-7CDD92182FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="120" windowWidth="21180" windowHeight="13665" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="615" yWindow="330" windowWidth="24330" windowHeight="13665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OVERALL" sheetId="29" r:id="rId1"/>
@@ -2137,6 +2137,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="15" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2148,63 +2157,6 @@
     </xf>
     <xf numFmtId="14" fontId="16" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="20" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2250,6 +2202,54 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="15" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2722,7 +2722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5CD2D7D-160B-4F5B-BCD4-B88367B920F0}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -3354,7 +3354,7 @@
     <mergeCell ref="H1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -21339,7 +21339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A1EE897-404D-4ADC-856A-1E864FE4E3AA}">
   <dimension ref="A1:BB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="BB25" sqref="BB25"/>
     </sheetView>
   </sheetViews>
@@ -21387,228 +21387,228 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:54" s="1" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="238" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="225"/>
-      <c r="D1" s="228" t="s">
+      <c r="B1" s="239"/>
+      <c r="C1" s="244"/>
+      <c r="D1" s="247" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="213" t="s">
+      <c r="E1" s="216" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="214"/>
-      <c r="G1" s="213" t="s">
+      <c r="F1" s="217"/>
+      <c r="G1" s="216" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="214"/>
-      <c r="I1" s="213" t="s">
+      <c r="H1" s="217"/>
+      <c r="I1" s="216" t="s">
         <v>47</v>
       </c>
-      <c r="J1" s="214"/>
-      <c r="K1" s="213" t="s">
+      <c r="J1" s="217"/>
+      <c r="K1" s="216" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="214"/>
-      <c r="M1" s="213" t="s">
+      <c r="L1" s="217"/>
+      <c r="M1" s="216" t="s">
         <v>80</v>
       </c>
-      <c r="N1" s="214"/>
-      <c r="O1" s="213" t="s">
+      <c r="N1" s="217"/>
+      <c r="O1" s="216" t="s">
         <v>94</v>
       </c>
-      <c r="P1" s="214"/>
-      <c r="Q1" s="213" t="s">
+      <c r="P1" s="217"/>
+      <c r="Q1" s="216" t="s">
         <v>99</v>
       </c>
-      <c r="R1" s="214"/>
-      <c r="S1" s="213" t="s">
+      <c r="R1" s="217"/>
+      <c r="S1" s="216" t="s">
         <v>103</v>
       </c>
-      <c r="T1" s="214"/>
-      <c r="U1" s="213" t="s">
+      <c r="T1" s="217"/>
+      <c r="U1" s="216" t="s">
         <v>107</v>
       </c>
-      <c r="V1" s="214"/>
-      <c r="W1" s="213" t="s">
+      <c r="V1" s="217"/>
+      <c r="W1" s="216" t="s">
         <v>109</v>
       </c>
-      <c r="X1" s="214"/>
-      <c r="Y1" s="213" t="s">
+      <c r="X1" s="217"/>
+      <c r="Y1" s="216" t="s">
         <v>110</v>
       </c>
-      <c r="Z1" s="214"/>
-      <c r="AA1" s="213" t="s">
+      <c r="Z1" s="217"/>
+      <c r="AA1" s="216" t="s">
         <v>119</v>
       </c>
-      <c r="AB1" s="214"/>
-      <c r="AC1" s="213" t="s">
+      <c r="AB1" s="217"/>
+      <c r="AC1" s="216" t="s">
         <v>124</v>
       </c>
-      <c r="AD1" s="214"/>
-      <c r="AE1" s="213" t="s">
+      <c r="AD1" s="217"/>
+      <c r="AE1" s="216" t="s">
         <v>126</v>
       </c>
-      <c r="AF1" s="214"/>
-      <c r="AG1" s="213" t="s">
+      <c r="AF1" s="217"/>
+      <c r="AG1" s="216" t="s">
         <v>127</v>
       </c>
-      <c r="AH1" s="214"/>
-      <c r="AI1" s="213" t="s">
+      <c r="AH1" s="217"/>
+      <c r="AI1" s="216" t="s">
         <v>129</v>
       </c>
-      <c r="AJ1" s="214"/>
-      <c r="AK1" s="213" t="s">
+      <c r="AJ1" s="217"/>
+      <c r="AK1" s="216" t="s">
         <v>130</v>
       </c>
-      <c r="AL1" s="214"/>
-      <c r="AM1" s="213" t="s">
+      <c r="AL1" s="217"/>
+      <c r="AM1" s="216" t="s">
         <v>132</v>
       </c>
-      <c r="AN1" s="214"/>
-      <c r="AO1" s="213" t="s">
+      <c r="AN1" s="217"/>
+      <c r="AO1" s="216" t="s">
         <v>133</v>
       </c>
-      <c r="AP1" s="214"/>
-      <c r="AQ1" s="230" t="s">
+      <c r="AP1" s="217"/>
+      <c r="AQ1" s="235" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="239" t="s">
+      <c r="AR1" s="223" t="s">
         <v>125</v>
       </c>
       <c r="AS1" s="121"/>
-      <c r="AT1" s="242" t="s">
+      <c r="AT1" s="226" t="s">
         <v>117</v>
       </c>
-      <c r="AU1" s="243"/>
-      <c r="AV1" s="243"/>
-      <c r="AW1" s="244"/>
-      <c r="AX1" s="233" t="s">
+      <c r="AU1" s="227"/>
+      <c r="AV1" s="227"/>
+      <c r="AW1" s="228"/>
+      <c r="AX1" s="213" t="s">
         <v>123</v>
       </c>
-      <c r="AY1" s="236" t="s">
+      <c r="AY1" s="220" t="s">
         <v>118</v>
       </c>
-      <c r="AZ1" s="237"/>
-      <c r="BA1" s="237"/>
-      <c r="BB1" s="238"/>
+      <c r="AZ1" s="221"/>
+      <c r="BA1" s="221"/>
+      <c r="BB1" s="222"/>
     </row>
     <row r="2" spans="1:54" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="221"/>
-      <c r="B2" s="222"/>
-      <c r="C2" s="226"/>
-      <c r="D2" s="229"/>
-      <c r="E2" s="215">
+      <c r="A2" s="240"/>
+      <c r="B2" s="241"/>
+      <c r="C2" s="245"/>
+      <c r="D2" s="248"/>
+      <c r="E2" s="218">
         <v>45418</v>
       </c>
-      <c r="F2" s="216"/>
-      <c r="G2" s="217">
+      <c r="F2" s="219"/>
+      <c r="G2" s="249">
         <v>45425</v>
       </c>
-      <c r="H2" s="218"/>
-      <c r="I2" s="217">
+      <c r="H2" s="250"/>
+      <c r="I2" s="249">
         <v>45432</v>
       </c>
-      <c r="J2" s="218"/>
-      <c r="K2" s="217">
+      <c r="J2" s="250"/>
+      <c r="K2" s="249">
         <v>45439</v>
       </c>
-      <c r="L2" s="218"/>
-      <c r="M2" s="217">
+      <c r="L2" s="250"/>
+      <c r="M2" s="249">
         <v>45446</v>
       </c>
-      <c r="N2" s="218"/>
-      <c r="O2" s="217">
+      <c r="N2" s="250"/>
+      <c r="O2" s="249">
         <v>45453</v>
       </c>
-      <c r="P2" s="218"/>
-      <c r="Q2" s="217">
+      <c r="P2" s="250"/>
+      <c r="Q2" s="249">
         <v>45460</v>
       </c>
-      <c r="R2" s="218"/>
-      <c r="S2" s="217">
+      <c r="R2" s="250"/>
+      <c r="S2" s="249">
         <v>45467</v>
       </c>
-      <c r="T2" s="218"/>
-      <c r="U2" s="217">
+      <c r="T2" s="250"/>
+      <c r="U2" s="249">
         <v>45474</v>
       </c>
-      <c r="V2" s="218"/>
-      <c r="W2" s="217">
+      <c r="V2" s="250"/>
+      <c r="W2" s="249">
         <v>45481</v>
       </c>
-      <c r="X2" s="218"/>
-      <c r="Y2" s="217">
+      <c r="X2" s="250"/>
+      <c r="Y2" s="249">
         <v>45488</v>
       </c>
-      <c r="Z2" s="218"/>
-      <c r="AA2" s="215">
+      <c r="Z2" s="250"/>
+      <c r="AA2" s="218">
         <v>45495</v>
       </c>
-      <c r="AB2" s="216"/>
-      <c r="AC2" s="215">
+      <c r="AB2" s="219"/>
+      <c r="AC2" s="218">
         <v>45502</v>
       </c>
-      <c r="AD2" s="216"/>
-      <c r="AE2" s="215">
+      <c r="AD2" s="219"/>
+      <c r="AE2" s="218">
         <v>45509</v>
       </c>
-      <c r="AF2" s="216"/>
-      <c r="AG2" s="215">
+      <c r="AF2" s="219"/>
+      <c r="AG2" s="218">
         <v>45516</v>
       </c>
-      <c r="AH2" s="216"/>
-      <c r="AI2" s="215">
+      <c r="AH2" s="219"/>
+      <c r="AI2" s="218">
         <v>45523</v>
       </c>
-      <c r="AJ2" s="216"/>
-      <c r="AK2" s="215">
+      <c r="AJ2" s="219"/>
+      <c r="AK2" s="218">
         <v>45530</v>
       </c>
-      <c r="AL2" s="216"/>
-      <c r="AM2" s="215">
+      <c r="AL2" s="219"/>
+      <c r="AM2" s="218">
         <v>45537</v>
       </c>
-      <c r="AN2" s="216"/>
-      <c r="AO2" s="215">
+      <c r="AN2" s="219"/>
+      <c r="AO2" s="218">
         <v>45544</v>
       </c>
-      <c r="AP2" s="216"/>
-      <c r="AQ2" s="231"/>
-      <c r="AR2" s="240"/>
+      <c r="AP2" s="219"/>
+      <c r="AQ2" s="236"/>
+      <c r="AR2" s="224"/>
       <c r="AS2" s="121"/>
-      <c r="AT2" s="245" t="s">
+      <c r="AT2" s="229" t="s">
         <v>98</v>
       </c>
-      <c r="AU2" s="247" t="s">
+      <c r="AU2" s="231" t="s">
         <v>116</v>
       </c>
-      <c r="AV2" s="247" t="s">
+      <c r="AV2" s="231" t="s">
         <v>43</v>
       </c>
-      <c r="AW2" s="249" t="s">
+      <c r="AW2" s="233" t="s">
         <v>70</v>
       </c>
-      <c r="AX2" s="234"/>
-      <c r="AY2" s="233" t="s">
+      <c r="AX2" s="214"/>
+      <c r="AY2" s="213" t="s">
         <v>98</v>
       </c>
-      <c r="AZ2" s="233" t="s">
+      <c r="AZ2" s="213" t="s">
         <v>116</v>
       </c>
-      <c r="BA2" s="233" t="s">
+      <c r="BA2" s="213" t="s">
         <v>43</v>
       </c>
-      <c r="BB2" s="233" t="s">
+      <c r="BB2" s="213" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:54" s="1" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="223"/>
-      <c r="B3" s="224"/>
-      <c r="C3" s="227"/>
-      <c r="D3" s="229"/>
+      <c r="A3" s="242"/>
+      <c r="B3" s="243"/>
+      <c r="C3" s="246"/>
+      <c r="D3" s="248"/>
       <c r="E3" s="60" t="s">
         <v>28</v>
       </c>
@@ -21723,18 +21723,18 @@
       <c r="AP3" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="AQ3" s="232"/>
-      <c r="AR3" s="241"/>
+      <c r="AQ3" s="237"/>
+      <c r="AR3" s="225"/>
       <c r="AS3" s="121"/>
-      <c r="AT3" s="246"/>
-      <c r="AU3" s="248"/>
-      <c r="AV3" s="248"/>
-      <c r="AW3" s="250"/>
-      <c r="AX3" s="235"/>
-      <c r="AY3" s="234"/>
-      <c r="AZ3" s="234"/>
-      <c r="BA3" s="234"/>
-      <c r="BB3" s="235"/>
+      <c r="AT3" s="230"/>
+      <c r="AU3" s="232"/>
+      <c r="AV3" s="232"/>
+      <c r="AW3" s="234"/>
+      <c r="AX3" s="215"/>
+      <c r="AY3" s="214"/>
+      <c r="AZ3" s="214"/>
+      <c r="BA3" s="214"/>
+      <c r="BB3" s="215"/>
     </row>
     <row r="4" spans="1:54" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="64" t="s">
@@ -24141,28 +24141,22 @@
     <sortCondition ref="AR4:AR20"/>
   </sortState>
   <mergeCells count="54">
-    <mergeCell ref="AX1:AX3"/>
-    <mergeCell ref="AM1:AN1"/>
-    <mergeCell ref="AM2:AN2"/>
-    <mergeCell ref="AY1:BB1"/>
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BA2:BA3"/>
-    <mergeCell ref="BB2:BB3"/>
-    <mergeCell ref="AR1:AR3"/>
-    <mergeCell ref="AT1:AW1"/>
-    <mergeCell ref="AT2:AT3"/>
-    <mergeCell ref="AU2:AU3"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AQ1:AQ3"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AO1:AP1"/>
-    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="A1:B3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="D1:D3"/>
@@ -24179,22 +24173,28 @@
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AQ1:AQ3"/>
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AO1:AP1"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AX1:AX3"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AY1:BB1"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BA2:BA3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="AR1:AR3"/>
+    <mergeCell ref="AT1:AW1"/>
+    <mergeCell ref="AT2:AT3"/>
+    <mergeCell ref="AU2:AU3"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AW2:AW3"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>